<commit_message>
ignored order.xlsx and added double colons
</commit_message>
<xml_diff>
--- a/database/orders.xlsx
+++ b/database/orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,10 +496,8 @@
           <t>2024-10-04 08:47 AM</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2400</t>
-        </is>
+      <c r="E2" t="n">
+        <v>2400</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -507,10 +505,46 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>483843992</t>
-        </is>
+      <c r="H2" t="n">
+        <v>483843992</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>u6745</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Shahroz Ansari</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'Classic Burger': 1, 'Cheese Burger': 1, 'Chicken Nuggets': 1, 'Onion Rings': 1, 'French Fries': 1, 'Ham Sandwich': 1}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-10-06 02:59 PM</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2550</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Bakers street 29</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>No sauce, extra cheese</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3444231978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>